<commit_message>
ci: fixed some typoes
</commit_message>
<xml_diff>
--- a/LF/TAS/Cote d'Ivoire/Fev 2023/ci_202302_lf_tas1_2_partcipants.xlsx
+++ b/LF/TAS/Cote d'Ivoire/Fev 2023/ci_202302_lf_tas1_2_partcipants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\WHO\dsa-forms\LF\TAS\Cote d'Ivoire\Fev 2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEBC2449-DFEA-4364-BA43-BE6369B770E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{643C333C-E6C0-48C9-AF4D-4193BD6E1AB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -363,7 +363,7 @@
     <t>ci_202302_lf_tas1_2_partcipants</t>
   </si>
   <si>
-    <t>(2023 Dev) 2. TAS1 FL - Participants</t>
+    <t>(2023 Fev) 2. TAS1 FL - Participants</t>
   </si>
 </sst>
 </file>

</xml_diff>